<commit_message>
ajout de lien dans analyse SEO
</commit_message>
<xml_diff>
--- a/analyseSEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/analyseSEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassrooms\Projet_4_optimise\analyseSEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A69FF3-0F9D-462A-8CE1-6844544F78A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B60FB5-64E0-48B4-B902-B36E532DEF98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
   <si>
     <t>Categorie</t>
   </si>
@@ -305,13 +305,19 @@
   </si>
   <si>
     <t>Insérer "defer" dans les balises js</t>
+  </si>
+  <si>
+    <t>Cours SEO</t>
+  </si>
+  <si>
+    <t>Site Ionos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -333,6 +339,12 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -405,10 +417,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -441,8 +454,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -659,7 +679,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -729,8 +749,8 @@
       <c r="E2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>88</v>
+      <c r="F2" s="16" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -749,7 +769,7 @@
       <c r="E3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="16" t="s">
         <v>89</v>
       </c>
     </row>
@@ -769,7 +789,7 @@
       <c r="E4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -789,7 +809,7 @@
       <c r="E5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -809,7 +829,7 @@
       <c r="E6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="16" t="s">
         <v>9</v>
       </c>
     </row>
@@ -829,7 +849,7 @@
       <c r="E7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -849,7 +869,7 @@
       <c r="E8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="16" t="s">
         <v>86</v>
       </c>
     </row>
@@ -869,7 +889,7 @@
       <c r="E9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="16" t="s">
         <v>9</v>
       </c>
     </row>
@@ -889,7 +909,7 @@
       <c r="E10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="17" t="s">
         <v>33</v>
       </c>
     </row>
@@ -909,8 +929,8 @@
       <c r="E11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>9</v>
+      <c r="F11" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -929,7 +949,7 @@
       <c r="E12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -949,7 +969,7 @@
       <c r="E13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -969,7 +989,7 @@
       <c r="E14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="16" t="s">
         <v>87</v>
       </c>
     </row>
@@ -989,7 +1009,7 @@
       <c r="E15" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1009,7 +1029,7 @@
       <c r="E16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="16" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1029,8 +1049,8 @@
       <c r="E17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>9</v>
+      <c r="F17" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1049,7 +1069,7 @@
       <c r="E18" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="16" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1069,7 +1089,7 @@
       <c r="E19" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="17" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1089,7 +1109,7 @@
       <c r="E20" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="17" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2232,7 +2252,28 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{EBC69D24-BB29-49C5-AC4D-8328ACCC3942}"/>
+    <hyperlink ref="F10" r:id="rId2" xr:uid="{9082B6D6-963F-441C-85B8-7C9D8C7C6411}"/>
+    <hyperlink ref="F13" r:id="rId3" xr:uid="{7F2180B3-264E-41C4-BD77-24B93C5855A0}"/>
+    <hyperlink ref="F15" r:id="rId4" xr:uid="{2B6FA34A-FD03-4386-9666-79D4458A2B5C}"/>
+    <hyperlink ref="F19" r:id="rId5" xr:uid="{E6C708FF-83CD-4722-85D1-1AF93AF6259B}"/>
+    <hyperlink ref="F17" r:id="rId6" xr:uid="{06B0AE2B-B893-47AF-873B-44626B66D620}"/>
+    <hyperlink ref="F16" r:id="rId7" xr:uid="{CCABF3C2-A457-46F4-9F82-1CA752006196}"/>
+    <hyperlink ref="F14" r:id="rId8" xr:uid="{46969FC9-A714-4259-9158-D66ECF21F2C4}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{68120386-390C-43A5-AD0F-122BF7AFC829}"/>
+    <hyperlink ref="F4" r:id="rId10" xr:uid="{14EBF99C-FD65-4F38-B058-7A09059FCAF2}"/>
+    <hyperlink ref="F6" r:id="rId11" xr:uid="{3FEEFA3A-A8E5-41EF-B5B0-118A499FF0E4}"/>
+    <hyperlink ref="F7" r:id="rId12" xr:uid="{FBA0B080-D223-4DA8-B7D4-CAC9E10D133D}"/>
+    <hyperlink ref="F18" r:id="rId13" xr:uid="{1AB70AE3-4713-45C6-80F5-BAB6699B161F}"/>
+    <hyperlink ref="F20" r:id="rId14" xr:uid="{252CD4BA-CA56-4B03-B794-0045AFA22BBB}"/>
+    <hyperlink ref="F9" r:id="rId15" xr:uid="{1162BB6B-E52A-4FC9-A1D6-8C457DEDBDF6}"/>
+    <hyperlink ref="F2" r:id="rId16" xr:uid="{024DA6DE-4EA9-46B2-9C73-2E97D4AECFD0}"/>
+    <hyperlink ref="F5" r:id="rId17" xr:uid="{F9A91D0C-B649-4D36-BA09-150497AAC71A}"/>
+    <hyperlink ref="F12" r:id="rId18" xr:uid="{3B8BD12A-0074-4278-977B-4DF6F52CD5F0}"/>
+    <hyperlink ref="F11" r:id="rId19" xr:uid="{74980C35-DBB9-47AA-AD2D-A94EB512F2C2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>